<commit_message>
Update profit files after running on 2025-09-04
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,19 @@
         <v>0.8838192269725232</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>09/04/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.1190458572798798</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.8809541427201202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-05
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,19 @@
         <v>0.8809541427201202</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1196901916565665</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8803098083434335</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-06
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,19 @@
         <v>0.8803098083434335</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>09/06/2025</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1259940523634941</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.8740059476365059</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-07
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,6 +502,19 @@
         <v>0.8740059476365059</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>09/07/2025</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1257222453734942</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.8742777546265058</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-08
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,6 +515,19 @@
         <v>0.8742777546265058</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>09/08/2025</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1229112743299529</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.8770887256700471</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-09
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,6 +528,19 @@
         <v>0.8770887256700471</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>09/09/2025</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1246141075485167</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.8753858924514833</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-10
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +541,19 @@
         <v>0.8753858924514833</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>09/10/2025</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1250185577428985</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8749814422571015</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-11
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,19 @@
         <v>0.8749814422571015</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>09/11/2025</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.1236841051452084</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.8763158948547916</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-12
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,6 +567,19 @@
         <v>0.8763158948547916</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>09/12/2025</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.1205199642338759</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8794800357661241</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-13
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -580,6 +580,19 @@
         <v>0.8794800357661241</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>09/13/2025</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1167782903132609</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8832217096867391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-14
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,6 +593,19 @@
         <v>0.8832217096867391</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>09/14/2025</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.1222829562546641</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8777170437453359</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-15
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,6 +606,19 @@
         <v>0.8777170437453359</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>09/15/2025</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.1268672426830251</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8731327573169749</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-16
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,6 +619,19 @@
         <v>0.8731327573169749</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>09/16/2025</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.1244621484369293</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.8755378515630707</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-17
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -632,6 +632,19 @@
         <v>0.8755378515630707</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>09/17/2025</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.1245762204778458</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8754237795221542</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-18
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -645,6 +645,19 @@
         <v>0.8754237795221542</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>09/18/2025</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.1212928116459102</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.8787071883540898</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-19
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -658,6 +658,19 @@
         <v>0.8787071883540898</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>09/19/2025</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.1241833645951854</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8758166354048146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-20
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,6 +671,19 @@
         <v>0.8758166354048146</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>09/20/2025</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.1258563147191275</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.8741436852808725</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-21
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,6 +684,19 @@
         <v>0.8741436852808725</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>09/21/2025</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.1307131026099658</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.8692868973900342</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-22
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -697,6 +697,19 @@
         <v>0.8692868973900342</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>09/22/2025</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1347731634554507</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.8652268365445493</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-23
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -710,6 +710,19 @@
         <v>0.8652268365445493</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>09/23/2025</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.1311905007115779</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.8688094992884221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-24
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -723,6 +723,19 @@
         <v>0.8688094992884221</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>09/24/2025</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.1319396418060274</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.8680603581939726</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-25
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -736,6 +736,19 @@
         <v>0.8680603581939726</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>09/25/2025</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.1344413231227061</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.8655586768772939</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-26
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -749,6 +749,19 @@
         <v>0.8655586768772939</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>09/26/2025</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.1317299397691639</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.8682700602308361</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-27
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -762,6 +762,19 @@
         <v>0.8682700602308361</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>09/27/2025</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.1324659859615432</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.8675340140384568</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-28
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,6 +775,19 @@
         <v>0.8675340140384568</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>09/28/2025</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.1383344084454727</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.8616655915545273</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-29
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -788,6 +788,19 @@
         <v>0.8616655915545273</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>09/29/2025</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.1388883331783817</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.8611116668216183</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-09-30
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -801,6 +801,19 @@
         <v>0.8611116668216183</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>09/30/2025</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.1412270494756673</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.8587729505243327</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-01
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -814,6 +814,19 @@
         <v>0.8587729505243327</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>10/01/2025</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.1405966619741709</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.8594033380258291</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-02
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -827,6 +827,19 @@
         <v>0.8594033380258291</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>10/02/2025</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.1380907263517728</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.8619092736482272</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-03
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -840,6 +840,19 @@
         <v>0.8619092736482272</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>10/03/2025</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.1416568838977773</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.8583431161022227</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-04
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -853,6 +853,19 @@
         <v>0.8583431161022227</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>10/04/2025</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.1465718972668775</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.8534281027331225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-05
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -866,6 +866,19 @@
         <v>0.8534281027331225</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>10/05/2025</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.1522908069229351</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.8477091930770649</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-06
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -879,6 +879,19 @@
         <v>0.8477091930770649</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>10/06/2025</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.1521778353556913</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.8478221646443087</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-07
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -892,6 +892,19 @@
         <v>0.8478221646443087</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>10/07/2025</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.151313202125494</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.848686797874506</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-08
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -905,6 +905,19 @@
         <v>0.848686797874506</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>10/08/2025</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.1528034018842741</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.8471965981157259</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-09
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -918,6 +918,19 @@
         <v>0.8471965981157259</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>10/09/2025</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.1560717738048621</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.8439282261951379</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-10
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -931,6 +931,19 @@
         <v>0.8439282261951379</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>10/10/2025</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.1531112533627095</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.8468887466372905</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-11
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -944,6 +944,19 @@
         <v>0.8468887466372905</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>10/11/2025</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.1742587702834341</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.8257412297165659</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-12
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -957,6 +957,19 @@
         <v>0.8257412297165659</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.1777389139054508</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.8222610860945492</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-13
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -970,6 +970,19 @@
         <v>0.8222610860945492</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>10/13/2025</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.1714181428297508</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.8285818571702492</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-14
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -983,6 +983,19 @@
         <v>0.8285818571702492</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>10/14/2025</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.1768496803993662</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.8231503196006338</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-15
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -996,6 +996,19 @@
         <v>0.8231503196006338</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>10/15/2025</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.1768812452900025</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.8231187547099975</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-16
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1009,6 +1009,19 @@
         <v>0.8231187547099975</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>10/16/2025</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.1765432923704638</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.8234567076295362</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-17
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1022,6 +1022,19 @@
         <v>0.8234567076295362</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>10/17/2025</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.1864789165136171</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.8135210834863829</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-18
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1035,6 +1035,19 @@
         <v>0.8135210834863829</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>10/18/2025</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.1870601725438363</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.8129398274561637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-19
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1048,6 +1048,19 @@
         <v>0.8129398274561637</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>10/19/2025</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.1940814947980256</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.8059185052019744</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-20
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1061,6 +1061,19 @@
         <v>0.8059185052019744</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>10/20/2025</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.1910841114775904</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.8089158885224096</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-21
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1074,6 +1074,19 @@
         <v>0.8089158885224096</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>10/21/2025</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.1928588791428576</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.8071411208571424</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-22
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1087,6 +1087,19 @@
         <v>0.8071411208571424</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>10/22/2025</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.1958319825464067</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.8041680174535933</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-23
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1100,6 +1100,19 @@
         <v>0.8041680174535933</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>10/23/2025</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.196346158260441</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.803653841739559</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-24
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1113,6 +1113,19 @@
         <v>0.803653841739559</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>10/24/2025</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.1958495701456533</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.8041504298543467</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-25
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1126,6 +1126,19 @@
         <v>0.8041504298543467</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>10/25/2025</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.190092683663864</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.809907316336136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-26
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1139,6 +1139,19 @@
         <v>0.809907316336136</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>10/26/2025</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.1833298628465994</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.8166701371534006</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-27
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1152,6 +1152,19 @@
         <v>0.8166701371534006</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>10/27/2025</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.189372928692943</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.810627071307057</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-28
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1165,6 +1165,19 @@
         <v>0.810627071307057</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>10/28/2025</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.1865144124783668</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.8134855875216332</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-29
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1178,6 +1178,19 @@
         <v>0.8134855875216332</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>10/29/2025</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.1825660000012012</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.8174339999987988</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-30
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1191,6 +1191,19 @@
         <v>0.8174339999987988</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>10/30/2025</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.1871352070866719</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.8128647929133281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-10-31
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1204,6 +1204,19 @@
         <v>0.8128647929133281</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>10/31/2025</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.1918410875229571</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.8081589124770429</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-01
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1217,6 +1217,19 @@
         <v>0.8081589124770429</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>11/01/2025</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.1915577992289118</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.8084422007710882</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-02
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1230,6 +1230,19 @@
         <v>0.8084422007710882</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>11/02/2025</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.1979663639690586</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.8020336360309414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-03
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1243,6 +1243,19 @@
         <v>0.8020336360309414</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>11/03/2025</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.2058740788361836</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.7941259211638164</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-04
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1256,6 +1256,19 @@
         <v>0.7941259211638164</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.2154778411495352</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.7845221588504648</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-05
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1269,6 +1269,19 @@
         <v>0.7845221588504648</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>11/05/2025</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.2116545376383344</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.7883454623616656</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-06
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1282,6 +1282,19 @@
         <v>0.7883454623616656</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>11/06/2025</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.2107717439314687</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.7892282560685313</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-07
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1295,6 +1295,19 @@
         <v>0.7892282560685313</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>11/07/2025</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.1940232686290251</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.8059767313709749</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-08
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1308,6 +1308,19 @@
         <v>0.8059767313709749</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>11/08/2025</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.185766309476215</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.814233690523785</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-09
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1321,6 +1321,19 @@
         <v>0.814233690523785</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>11/09/2025</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.1958362470302913</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.8041637529697087</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-10
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1334,6 +1334,19 @@
         <v>0.8041637529697087</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>11/10/2025</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.1940694112342378</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.8059305887657622</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-11
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1347,6 +1347,19 @@
         <v>0.8059305887657622</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>11/11/2025</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.1975015291293336</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.8024984708706664</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-12
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1360,6 +1360,19 @@
         <v>0.8024984708706664</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.2016542154360835</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.7983457845639165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-13
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1373,6 +1373,19 @@
         <v>0.7983457845639165</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>11/13/2025</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.1975578351244442</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.8024421648755558</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-14
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1386,6 +1386,19 @@
         <v>0.8024421648755558</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>11/14/2025</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.2019497281731677</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.7980502718268323</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-15
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1399,6 +1399,19 @@
         <v>0.7980502718268323</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>11/15/2025</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.201282096967901</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.798717903032099</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-16
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1412,6 +1412,19 @@
         <v>0.798717903032099</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>11/16/2025</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.2029201483094979</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.7970798516905021</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-17
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1425,6 +1425,19 @@
         <v>0.7970798516905021</v>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>11/17/2025</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.2014044958689747</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.7985955041310253</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-18
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1438,6 +1438,19 @@
         <v>0.7985955041310253</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>11/18/2025</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.2054993753108948</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.7945006246891052</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-19
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1451,6 +1451,19 @@
         <v>0.7945006246891052</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>11/19/2025</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.2041669959013599</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.7958330040986401</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-20
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1464,6 +1464,19 @@
         <v>0.7958330040986401</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>11/20/2025</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.2044597188475565</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.7955402811524435</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-21
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1477,6 +1477,19 @@
         <v>0.7955402811524435</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>11/21/2025</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.2092672469831965</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.7907327530168035</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-22
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1490,6 +1490,19 @@
         <v>0.7907327530168035</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>11/22/2025</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.2103874149996593</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.7896125850003407</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-23
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1503,6 +1503,19 @@
         <v>0.7896125850003407</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>11/23/2025</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.2078408625589678</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.7921591374410322</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-24
</commit_message>
<xml_diff>
--- a/data/allocation.xlsx
+++ b/data/allocation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1516,6 +1516,19 @@
         <v>0.7921591374410322</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>11/24/2025</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0.2067077544858842</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.7932922455141158</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>